<commit_message>
Added info to excel file
</commit_message>
<xml_diff>
--- a/k.xlsx
+++ b/k.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github sdet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1211502F-ED99-4A6C-87D6-E43D490A037A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,73 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Types of Testing Documents</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Test policy</t>
+  </si>
+  <si>
+    <t>It is a high-level document which describes principles, methods and all the important testing goals of the organization.</t>
+  </si>
+  <si>
+    <t>Test strategy</t>
+  </si>
+  <si>
+    <t>A high-level document which identifies the Test Levels (types) to be executed for the project.</t>
+  </si>
+  <si>
+    <t>Test plan</t>
+  </si>
+  <si>
+    <t>A test plan is a complete planning document which contains the scope, approach, resources, schedule, etc. of testing activities.</t>
+  </si>
+  <si>
+    <t>Requirements Traceability Matrix</t>
+  </si>
+  <si>
+    <t>This is a document which connects the requirements to the test cases.</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Test scenario is an item or event of a software system which could be verified by one or more Test cases.</t>
+  </si>
+  <si>
+    <t>Test case</t>
+  </si>
+  <si>
+    <t>It is a group of input values, execution preconditions, expected execution postconditions and results. It is developed for a Test Scenario.</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Test Data is a data which exists before a test is executed. It used to execute the test case.</t>
+  </si>
+  <si>
+    <t>Defect Report</t>
+  </si>
+  <si>
+    <t>Defect report is a documented report of any flaw in a Software System which fails to perform its expected function.</t>
+  </si>
+  <si>
+    <t>Test summary report</t>
+  </si>
+  <si>
+    <t>Test summary report is a high-level document which summarizes testing activities conducted as well as the test result.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,15 +100,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +122,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +424,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="113.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>